<commit_message>
New sheet added to cover from 13 - 25 in SRS sheet
</commit_message>
<xml_diff>
--- a/Testing/Foodies_TC_Report.xlsx
+++ b/Testing/Foodies_TC_Report.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Analysis" sheetId="2" r:id="rId2"/>
+    <sheet name="13-25" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="68">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1673,26 +1674,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB303"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" customWidth="1"/>
     <col min="6" max="6" width="41" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" style="11" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="4" customFormat="1" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" s="4" customFormat="1" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1742,7 +1743,7 @@
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
     </row>
-    <row r="2" spans="1:28" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="75.599999999999994" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
@@ -1771,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="105" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
@@ -1800,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="90" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>23</v>
       </c>
@@ -1829,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="105" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>27</v>
       </c>
@@ -1858,7 +1859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="75" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>30</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="180" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="150" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>33</v>
       </c>
@@ -1916,7 +1917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="180" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="150" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>37</v>
       </c>
@@ -1945,7 +1946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="180" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="150" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>40</v>
       </c>
@@ -1974,7 +1975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="60" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>53</v>
       </c>
@@ -2004,7 +2005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="60" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>56</v>
       </c>
@@ -2034,7 +2035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="285" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="285" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>62</v>
       </c>
@@ -2066,7 +2067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -2082,7 +2083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -2098,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -2114,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -2130,7 +2131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -2145,7 +2146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -2160,7 +2161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -2175,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -2190,7 +2191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -2205,7 +2206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -2220,7 +2221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -2235,7 +2236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -2250,7 +2251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -2265,7 +2266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -2280,7 +2281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -2295,7 +2296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -2310,7 +2311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -2325,7 +2326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -2340,7 +2341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -2355,7 +2356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -2370,7 +2371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -2385,7 +2386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -2400,7 +2401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -2415,7 +2416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -2430,7 +2431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -2445,7 +2446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -2460,7 +2461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -2475,7 +2476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
@@ -2490,7 +2491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -2505,7 +2506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -2520,7 +2521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
@@ -2535,7 +2536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -2550,7 +2551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -2565,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -2580,7 +2581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -2595,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -2610,7 +2611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A49" s="10"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -2625,7 +2626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A50" s="10"/>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -2640,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A51" s="10"/>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
@@ -2655,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
@@ -2670,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A53" s="10"/>
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
@@ -2685,7 +2686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A54" s="10"/>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -2700,7 +2701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A55" s="10"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
@@ -2715,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A56" s="10"/>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -2730,7 +2731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A57" s="10"/>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
@@ -2745,7 +2746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A58" s="10"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -2760,7 +2761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A59" s="10"/>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -2775,7 +2776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
@@ -2790,7 +2791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A61" s="10"/>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
@@ -2805,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A62" s="10"/>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
@@ -2820,7 +2821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A63" s="10"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
@@ -2835,7 +2836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A64" s="10"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
@@ -2850,7 +2851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A65" s="10"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
@@ -2865,7 +2866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
@@ -2880,7 +2881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A67" s="10"/>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
@@ -2895,7 +2896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A68" s="10"/>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -2910,7 +2911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A69" s="10"/>
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
@@ -2925,7 +2926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A70" s="10"/>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
@@ -2940,7 +2941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A71" s="10"/>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
@@ -2955,7 +2956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A72" s="10"/>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
@@ -2970,7 +2971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A73" s="10"/>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
@@ -2985,7 +2986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A74" s="10"/>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
@@ -3000,7 +3001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
@@ -3015,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A76" s="10"/>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
@@ -3030,7 +3031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A77" s="10"/>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -3045,7 +3046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A78" s="10"/>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
@@ -3060,7 +3061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A79" s="10"/>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
@@ -3075,7 +3076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A80" s="10"/>
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
@@ -3090,7 +3091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A81" s="10"/>
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
@@ -3105,7 +3106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A82" s="10"/>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
@@ -3120,7 +3121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A83" s="10"/>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
@@ -3135,7 +3136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A84" s="10"/>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
@@ -3150,7 +3151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A85" s="10"/>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
@@ -3165,7 +3166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A86" s="10"/>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
@@ -3180,7 +3181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A87" s="10"/>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
@@ -3195,7 +3196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A88" s="10"/>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
@@ -3210,7 +3211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A89" s="10"/>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
@@ -3225,7 +3226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A90" s="10"/>
       <c r="B90" s="10"/>
       <c r="C90" s="10"/>
@@ -3240,7 +3241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A91" s="10"/>
       <c r="B91" s="10"/>
       <c r="C91" s="10"/>
@@ -3255,7 +3256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A92" s="10"/>
       <c r="B92" s="10"/>
       <c r="C92" s="10"/>
@@ -3270,7 +3271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A93" s="10"/>
       <c r="B93" s="10"/>
       <c r="C93" s="10"/>
@@ -3285,7 +3286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A94" s="10"/>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
@@ -3300,7 +3301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A95" s="10"/>
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
@@ -3315,7 +3316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A96" s="10"/>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
@@ -3330,7 +3331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A97" s="10"/>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
@@ -3345,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A98" s="10"/>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
@@ -3360,7 +3361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A99" s="10"/>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
@@ -3375,7 +3376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A100" s="10"/>
       <c r="B100" s="10"/>
       <c r="C100" s="10"/>
@@ -3390,7 +3391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A101" s="10"/>
       <c r="B101" s="10"/>
       <c r="C101" s="10"/>
@@ -3405,7 +3406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A102" s="10"/>
       <c r="B102" s="10"/>
       <c r="C102" s="10"/>
@@ -3420,7 +3421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A103" s="10"/>
       <c r="B103" s="10"/>
       <c r="C103" s="10"/>
@@ -3435,7 +3436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A104" s="10"/>
       <c r="B104" s="10"/>
       <c r="C104" s="10"/>
@@ -3450,7 +3451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A105" s="10"/>
       <c r="B105" s="10"/>
       <c r="C105" s="10"/>
@@ -3465,7 +3466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A106" s="10"/>
       <c r="B106" s="10"/>
       <c r="C106" s="10"/>
@@ -3480,7 +3481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A107" s="10"/>
       <c r="B107" s="10"/>
       <c r="C107" s="10"/>
@@ -3495,7 +3496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A108" s="10"/>
       <c r="B108" s="10"/>
       <c r="C108" s="10"/>
@@ -3510,7 +3511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A109" s="10"/>
       <c r="B109" s="10"/>
       <c r="C109" s="10"/>
@@ -3525,7 +3526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A110" s="10"/>
       <c r="B110" s="10"/>
       <c r="C110" s="10"/>
@@ -3540,7 +3541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A111" s="10"/>
       <c r="B111" s="10"/>
       <c r="C111" s="10"/>
@@ -3555,7 +3556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A112" s="10"/>
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
@@ -3570,7 +3571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A113" s="10"/>
       <c r="B113" s="10"/>
       <c r="C113" s="10"/>
@@ -3585,7 +3586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A114" s="10"/>
       <c r="B114" s="10"/>
       <c r="C114" s="10"/>
@@ -3600,7 +3601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A115" s="10"/>
       <c r="B115" s="10"/>
       <c r="C115" s="10"/>
@@ -3615,7 +3616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A116" s="10"/>
       <c r="B116" s="10"/>
       <c r="C116" s="10"/>
@@ -3630,7 +3631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A117" s="10"/>
       <c r="B117" s="10"/>
       <c r="C117" s="10"/>
@@ -3645,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A118" s="10"/>
       <c r="B118" s="10"/>
       <c r="C118" s="10"/>
@@ -3660,7 +3661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A119" s="10"/>
       <c r="B119" s="10"/>
       <c r="C119" s="10"/>
@@ -3675,7 +3676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A120" s="10"/>
       <c r="B120" s="10"/>
       <c r="C120" s="10"/>
@@ -3690,7 +3691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A121" s="10"/>
       <c r="B121" s="10"/>
       <c r="C121" s="10"/>
@@ -3705,7 +3706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A122" s="10"/>
       <c r="B122" s="10"/>
       <c r="C122" s="10"/>
@@ -3720,7 +3721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A123" s="10"/>
       <c r="B123" s="10"/>
       <c r="C123" s="10"/>
@@ -3735,7 +3736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A124" s="10"/>
       <c r="B124" s="10"/>
       <c r="C124" s="10"/>
@@ -3750,7 +3751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A125" s="10"/>
       <c r="B125" s="10"/>
       <c r="C125" s="10"/>
@@ -3765,7 +3766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A126" s="10"/>
       <c r="B126" s="10"/>
       <c r="C126" s="10"/>
@@ -3780,7 +3781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A127" s="10"/>
       <c r="B127" s="10"/>
       <c r="C127" s="10"/>
@@ -3795,7 +3796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A128" s="10"/>
       <c r="B128" s="10"/>
       <c r="C128" s="10"/>
@@ -3810,7 +3811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A129" s="10"/>
       <c r="B129" s="10"/>
       <c r="C129" s="10"/>
@@ -3825,7 +3826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A130" s="10"/>
       <c r="B130" s="10"/>
       <c r="C130" s="10"/>
@@ -3840,7 +3841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A131" s="10"/>
       <c r="B131" s="10"/>
       <c r="C131" s="10"/>
@@ -3855,7 +3856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A132" s="10"/>
       <c r="B132" s="10"/>
       <c r="C132" s="10"/>
@@ -3870,7 +3871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A133" s="10"/>
       <c r="B133" s="10"/>
       <c r="C133" s="10"/>
@@ -3885,7 +3886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A134" s="10"/>
       <c r="B134" s="10"/>
       <c r="C134" s="10"/>
@@ -3900,7 +3901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A135" s="10"/>
       <c r="B135" s="10"/>
       <c r="C135" s="10"/>
@@ -3915,7 +3916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A136" s="10"/>
       <c r="B136" s="10"/>
       <c r="C136" s="10"/>
@@ -3930,7 +3931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A137" s="10"/>
       <c r="B137" s="10"/>
       <c r="C137" s="10"/>
@@ -3945,7 +3946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A138" s="10"/>
       <c r="B138" s="10"/>
       <c r="C138" s="10"/>
@@ -3960,7 +3961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A139" s="10"/>
       <c r="B139" s="10"/>
       <c r="C139" s="10"/>
@@ -3975,7 +3976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A140" s="10"/>
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
@@ -3990,7 +3991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A141" s="10"/>
       <c r="B141" s="10"/>
       <c r="C141" s="10"/>
@@ -4005,7 +4006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A142" s="10"/>
       <c r="B142" s="10"/>
       <c r="C142" s="10"/>
@@ -4020,7 +4021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A143" s="10"/>
       <c r="B143" s="10"/>
       <c r="C143" s="10"/>
@@ -4035,7 +4036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A144" s="10"/>
       <c r="B144" s="10"/>
       <c r="C144" s="10"/>
@@ -4050,7 +4051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A145" s="10"/>
       <c r="B145" s="10"/>
       <c r="C145" s="10"/>
@@ -4065,7 +4066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A146" s="10"/>
       <c r="B146" s="10"/>
       <c r="C146" s="10"/>
@@ -4080,7 +4081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A147" s="10"/>
       <c r="B147" s="10"/>
       <c r="C147" s="10"/>
@@ -4095,7 +4096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A148" s="10"/>
       <c r="B148" s="10"/>
       <c r="C148" s="10"/>
@@ -4110,7 +4111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A149" s="10"/>
       <c r="B149" s="10"/>
       <c r="C149" s="10"/>
@@ -4125,7 +4126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A150" s="10"/>
       <c r="B150" s="10"/>
       <c r="C150" s="10"/>
@@ -4140,7 +4141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A151" s="10"/>
       <c r="B151" s="10"/>
       <c r="C151" s="10"/>
@@ -4155,7 +4156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A152" s="10"/>
       <c r="B152" s="10"/>
       <c r="C152" s="10"/>
@@ -4170,7 +4171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A153" s="10"/>
       <c r="B153" s="10"/>
       <c r="C153" s="10"/>
@@ -4185,7 +4186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A154" s="10"/>
       <c r="B154" s="10"/>
       <c r="C154" s="10"/>
@@ -4200,7 +4201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A155" s="10"/>
       <c r="B155" s="10"/>
       <c r="C155" s="10"/>
@@ -4215,7 +4216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A156" s="10"/>
       <c r="B156" s="10"/>
       <c r="C156" s="10"/>
@@ -4230,7 +4231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A157" s="10"/>
       <c r="B157" s="10"/>
       <c r="C157" s="10"/>
@@ -4245,7 +4246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A158" s="10"/>
       <c r="B158" s="10"/>
       <c r="C158" s="10"/>
@@ -4260,7 +4261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A159" s="10"/>
       <c r="B159" s="10"/>
       <c r="C159" s="10"/>
@@ -4275,7 +4276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A160" s="10"/>
       <c r="B160" s="10"/>
       <c r="C160" s="10"/>
@@ -4290,7 +4291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A161" s="10"/>
       <c r="B161" s="10"/>
       <c r="C161" s="10"/>
@@ -4305,7 +4306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A162" s="10"/>
       <c r="B162" s="10"/>
       <c r="C162" s="10"/>
@@ -4320,7 +4321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A163" s="10"/>
       <c r="B163" s="10"/>
       <c r="C163" s="10"/>
@@ -4335,7 +4336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A164" s="10"/>
       <c r="B164" s="10"/>
       <c r="C164" s="10"/>
@@ -4350,7 +4351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A165" s="10"/>
       <c r="B165" s="10"/>
       <c r="C165" s="10"/>
@@ -4365,7 +4366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A166" s="10"/>
       <c r="B166" s="10"/>
       <c r="C166" s="10"/>
@@ -4380,7 +4381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A167" s="10"/>
       <c r="B167" s="10"/>
       <c r="C167" s="10"/>
@@ -4395,7 +4396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A168" s="10"/>
       <c r="B168" s="10"/>
       <c r="C168" s="10"/>
@@ -4410,7 +4411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A169" s="10"/>
       <c r="B169" s="10"/>
       <c r="C169" s="10"/>
@@ -4425,7 +4426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A170" s="10"/>
       <c r="B170" s="10"/>
       <c r="C170" s="10"/>
@@ -4440,7 +4441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A171" s="10"/>
       <c r="B171" s="10"/>
       <c r="C171" s="10"/>
@@ -4455,7 +4456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A172" s="10"/>
       <c r="B172" s="10"/>
       <c r="C172" s="10"/>
@@ -4470,7 +4471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A173" s="10"/>
       <c r="B173" s="10"/>
       <c r="C173" s="10"/>
@@ -4485,7 +4486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A174" s="10"/>
       <c r="B174" s="10"/>
       <c r="C174" s="10"/>
@@ -4500,7 +4501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A175" s="10"/>
       <c r="B175" s="10"/>
       <c r="C175" s="10"/>
@@ -4515,7 +4516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A176" s="10"/>
       <c r="B176" s="10"/>
       <c r="C176" s="10"/>
@@ -4530,7 +4531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A177" s="10"/>
       <c r="B177" s="10"/>
       <c r="C177" s="10"/>
@@ -4545,7 +4546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A178" s="10"/>
       <c r="B178" s="10"/>
       <c r="C178" s="10"/>
@@ -4560,7 +4561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A179" s="10"/>
       <c r="B179" s="10"/>
       <c r="C179" s="10"/>
@@ -4575,7 +4576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A180" s="10"/>
       <c r="B180" s="10"/>
       <c r="C180" s="10"/>
@@ -4590,7 +4591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A181" s="10"/>
       <c r="B181" s="10"/>
       <c r="C181" s="10"/>
@@ -4605,7 +4606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A182" s="10"/>
       <c r="B182" s="10"/>
       <c r="C182" s="10"/>
@@ -4620,7 +4621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A183" s="10"/>
       <c r="B183" s="10"/>
       <c r="C183" s="10"/>
@@ -4635,7 +4636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A184" s="10"/>
       <c r="B184" s="10"/>
       <c r="C184" s="10"/>
@@ -4650,7 +4651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A185" s="10"/>
       <c r="B185" s="10"/>
       <c r="C185" s="10"/>
@@ -4665,7 +4666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A186" s="10"/>
       <c r="B186" s="10"/>
       <c r="C186" s="10"/>
@@ -4680,7 +4681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A187" s="10"/>
       <c r="B187" s="10"/>
       <c r="C187" s="10"/>
@@ -4695,7 +4696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A188" s="10"/>
       <c r="B188" s="10"/>
       <c r="C188" s="10"/>
@@ -4710,7 +4711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A189" s="10"/>
       <c r="B189" s="10"/>
       <c r="C189" s="10"/>
@@ -4725,7 +4726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A190" s="10"/>
       <c r="B190" s="10"/>
       <c r="C190" s="10"/>
@@ -4740,7 +4741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A191" s="10"/>
       <c r="B191" s="10"/>
       <c r="C191" s="10"/>
@@ -4755,7 +4756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A192" s="10"/>
       <c r="B192" s="10"/>
       <c r="C192" s="10"/>
@@ -4770,7 +4771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A193" s="10"/>
       <c r="B193" s="10"/>
       <c r="C193" s="10"/>
@@ -4785,7 +4786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A194" s="10"/>
       <c r="B194" s="10"/>
       <c r="C194" s="10"/>
@@ -4800,7 +4801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A195" s="10"/>
       <c r="B195" s="10"/>
       <c r="C195" s="10"/>
@@ -4815,7 +4816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A196" s="10"/>
       <c r="B196" s="10"/>
       <c r="C196" s="10"/>
@@ -4830,7 +4831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A197" s="10"/>
       <c r="B197" s="10"/>
       <c r="C197" s="10"/>
@@ -4845,7 +4846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A198" s="10"/>
       <c r="B198" s="10"/>
       <c r="C198" s="10"/>
@@ -4860,7 +4861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A199" s="10"/>
       <c r="B199" s="10"/>
       <c r="C199" s="10"/>
@@ -4875,7 +4876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A200" s="10"/>
       <c r="B200" s="10"/>
       <c r="C200" s="10"/>
@@ -4890,7 +4891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A201" s="10"/>
       <c r="B201" s="10"/>
       <c r="C201" s="10"/>
@@ -4905,7 +4906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A202" s="10"/>
       <c r="B202" s="10"/>
       <c r="C202" s="10"/>
@@ -4920,7 +4921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A203" s="10"/>
       <c r="B203" s="10"/>
       <c r="C203" s="10"/>
@@ -4935,7 +4936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A204" s="10"/>
       <c r="B204" s="10"/>
       <c r="C204" s="10"/>
@@ -4950,7 +4951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A205" s="10"/>
       <c r="B205" s="10"/>
       <c r="C205" s="10"/>
@@ -4965,7 +4966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A206" s="10"/>
       <c r="B206" s="10"/>
       <c r="C206" s="10"/>
@@ -4980,7 +4981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A207" s="10"/>
       <c r="B207" s="10"/>
       <c r="C207" s="10"/>
@@ -4995,7 +4996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A208" s="10"/>
       <c r="B208" s="10"/>
       <c r="C208" s="10"/>
@@ -5010,7 +5011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A209" s="10"/>
       <c r="B209" s="10"/>
       <c r="C209" s="10"/>
@@ -5025,7 +5026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A210" s="10"/>
       <c r="B210" s="10"/>
       <c r="C210" s="10"/>
@@ -5040,7 +5041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A211" s="10"/>
       <c r="B211" s="10"/>
       <c r="C211" s="10"/>
@@ -5055,7 +5056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A212" s="10"/>
       <c r="B212" s="10"/>
       <c r="C212" s="10"/>
@@ -5070,7 +5071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A213" s="10"/>
       <c r="B213" s="10"/>
       <c r="C213" s="10"/>
@@ -5085,7 +5086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A214" s="10"/>
       <c r="B214" s="10"/>
       <c r="C214" s="10"/>
@@ -5100,7 +5101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A215" s="10"/>
       <c r="B215" s="10"/>
       <c r="C215" s="10"/>
@@ -5115,7 +5116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A216" s="10"/>
       <c r="B216" s="10"/>
       <c r="C216" s="10"/>
@@ -5130,7 +5131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A217" s="10"/>
       <c r="B217" s="10"/>
       <c r="C217" s="10"/>
@@ -5145,7 +5146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A218" s="10"/>
       <c r="B218" s="10"/>
       <c r="C218" s="10"/>
@@ -5160,7 +5161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A219" s="10"/>
       <c r="B219" s="10"/>
       <c r="C219" s="10"/>
@@ -5175,7 +5176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A220" s="10"/>
       <c r="B220" s="10"/>
       <c r="C220" s="10"/>
@@ -5190,7 +5191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A221" s="10"/>
       <c r="B221" s="10"/>
       <c r="C221" s="10"/>
@@ -5205,7 +5206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A222" s="10"/>
       <c r="B222" s="10"/>
       <c r="C222" s="10"/>
@@ -5220,7 +5221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A223" s="10"/>
       <c r="B223" s="10"/>
       <c r="C223" s="10"/>
@@ -5235,7 +5236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A224" s="10"/>
       <c r="B224" s="10"/>
       <c r="C224" s="10"/>
@@ -5250,7 +5251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A225" s="10"/>
       <c r="B225" s="10"/>
       <c r="C225" s="10"/>
@@ -5265,7 +5266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A226" s="10"/>
       <c r="B226" s="10"/>
       <c r="C226" s="10"/>
@@ -5280,7 +5281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A227" s="10"/>
       <c r="B227" s="10"/>
       <c r="C227" s="10"/>
@@ -5295,7 +5296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A228" s="10"/>
       <c r="B228" s="10"/>
       <c r="C228" s="10"/>
@@ -5310,7 +5311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A229" s="10"/>
       <c r="B229" s="10"/>
       <c r="C229" s="10"/>
@@ -5325,7 +5326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A230" s="10"/>
       <c r="B230" s="10"/>
       <c r="C230" s="10"/>
@@ -5338,7 +5339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A231" s="10"/>
       <c r="B231" s="10"/>
       <c r="C231" s="10"/>
@@ -5351,7 +5352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A232" s="10"/>
       <c r="B232" s="10"/>
       <c r="C232" s="10"/>
@@ -5364,7 +5365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A233" s="10"/>
       <c r="B233" s="10"/>
       <c r="C233" s="10"/>
@@ -5377,7 +5378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A234" s="10"/>
       <c r="B234" s="10"/>
       <c r="C234" s="10"/>
@@ -5390,7 +5391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A235" s="10"/>
       <c r="B235" s="10"/>
       <c r="C235" s="10"/>
@@ -5403,7 +5404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A236" s="10"/>
       <c r="B236" s="10"/>
       <c r="C236" s="10"/>
@@ -5416,7 +5417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A237" s="10"/>
       <c r="B237" s="10"/>
       <c r="C237" s="10"/>
@@ -5429,7 +5430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A238" s="10"/>
       <c r="B238" s="10"/>
       <c r="C238" s="10"/>
@@ -5442,7 +5443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A239" s="10"/>
       <c r="B239" s="10"/>
       <c r="C239" s="10"/>
@@ -5455,7 +5456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A240" s="10"/>
       <c r="B240" s="10"/>
       <c r="C240" s="10"/>
@@ -5468,7 +5469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A241" s="10"/>
       <c r="B241" s="10"/>
       <c r="C241" s="10"/>
@@ -5481,7 +5482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A242" s="10"/>
       <c r="B242" s="10"/>
       <c r="C242" s="10"/>
@@ -5494,7 +5495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A243" s="10"/>
       <c r="B243" s="10"/>
       <c r="C243" s="10"/>
@@ -5507,7 +5508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:16" ht="15" x14ac:dyDescent="0.3">
       <c r="A244" s="10"/>
       <c r="B244" s="10"/>
       <c r="C244" s="10"/>
@@ -5520,297 +5521,297 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P245">
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P246">
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P247">
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P248">
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P249">
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P250">
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P251">
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P252">
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P253">
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P254">
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P255">
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P256">
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="257" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P257">
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="258" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P258">
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="259" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P259">
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="260" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P260">
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="261" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P261">
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="262" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P262">
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="263" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P263">
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="264" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P264">
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="265" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P265">
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="266" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P266">
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="267" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P267">
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="268" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P268">
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="269" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P269">
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="270" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P270">
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="271" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P271">
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="272" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P272">
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="273" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P273">
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="274" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P274">
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="275" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P275">
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="276" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P276">
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="277" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P277">
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="278" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P278">
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="279" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P279">
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="280" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P280">
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="281" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P281">
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="282" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P282">
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="283" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P283">
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="284" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P284">
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="285" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P285">
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="286" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P286">
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="287" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P287">
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="288" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P288">
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="289" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P289">
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="290" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P290">
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="291" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P291">
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="292" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P292">
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="293" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P293">
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="294" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P294">
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="295" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P295">
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="296" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P296">
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="297" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P297">
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="298" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P298">
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="299" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P299">
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="300" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P300">
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="301" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P301">
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="302" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P302">
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="303" spans="16:16" x14ac:dyDescent="0.3">
       <c r="P303">
         <v>1</v>
       </c>
@@ -5841,9 +5842,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -5851,7 +5852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
@@ -5859,7 +5860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -5872,7 +5873,7 @@
         <v>0.54545454545454541</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -5885,7 +5886,7 @@
         <v>0.45454545454545453</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -5898,7 +5899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -5915,4 +5916,81 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.21875" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" s="4" customFormat="1" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+    </row>
+    <row r="2" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>